<commit_message>
Updated hours, added comments
</commit_message>
<xml_diff>
--- a/doc/DD_Hours.xlsx
+++ b/doc/DD_Hours.xlsx
@@ -2,14 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Metagross\Documents\GitHub\Team-Faucet\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,27 +24,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Github Setup</t>
-  </si>
-  <si>
-    <t>Github Debug</t>
-  </si>
-  <si>
-    <t>Initial Code</t>
-  </si>
-  <si>
-    <t>total:</t>
-  </si>
-  <si>
-    <t>Further improvements</t>
-  </si>
-  <si>
-    <t>2018-3-1 Modification and addition of exit class</t>
-  </si>
-  <si>
-    <t>2018-3-8 Migration to unbroken Github</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Documentation/SA demo</t>
+  </si>
+  <si>
+    <t>Write Public functions, basic structure</t>
+  </si>
+  <si>
+    <t>Make inert obstacles</t>
+  </si>
+  <si>
+    <t>Make Simple Interactables</t>
+  </si>
+  <si>
+    <t>Make Level Exit/Dodo Egg</t>
+  </si>
+  <si>
+    <t>Make Optional Obstacles</t>
+  </si>
+  <si>
+    <t>Integrate other's parts that were not previously working</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Final testing and build</t>
+  </si>
+  <si>
+    <t>Github setup, Etc.</t>
   </si>
 </sst>
 </file>
@@ -357,46 +383,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>4</v>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1">
-        <f>SUM(B:B)</f>
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <f>B2-C2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <f>B3-C3</f>
+        <v>-12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -404,7 +443,14 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D9" si="0">B4-C4</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -412,7 +458,14 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -420,10 +473,95 @@
         <v>6</v>
       </c>
       <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
         <v>4</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D3:D10" si="1">B10-C10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <f>SUM(B2:B10)</f>
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:D11" si="2">SUM(C2:C10)</f>
+        <v>77</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>-17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated personal hour sheet
</commit_message>
<xml_diff>
--- a/doc/DD_Hours.xlsx
+++ b/doc/DD_Hours.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Metagross\Documents\GitHub\Team-Faucet\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Metagross\Documents\Homework\CS 383 Software Engineering\Group\Team-Faucet-2\Team-Faucet\Team-Faucet\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -386,7 +386,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +539,7 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <f t="shared" ref="D3:D10" si="1">B10-C10</f>
+        <f t="shared" ref="D10" si="1">B10-C10</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>